<commit_message>
check validate import excel + fix flow create booking ui
</commit_message>
<xml_diff>
--- a/AirlinesReservationSystem/uploads/flight_ticket_class_data.xlsx
+++ b/AirlinesReservationSystem/uploads/flight_ticket_class_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FBT\Kì 8\PRN231\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FBT\Kì 8\PRN231\PRN231Fall2024_SE1714_Group5_ARS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDB7D7B-D9E3-4AEF-B5F8-B47679BA3D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341420CC-6F34-46BA-942E-B696453FB151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>FlightNumber</t>
   </si>
@@ -58,19 +58,7 @@
     <t>VN4567</t>
   </si>
   <si>
-    <t>VN0003</t>
-  </si>
-  <si>
-    <t>VN0004</t>
-  </si>
-  <si>
-    <t>VN0005</t>
-  </si>
-  <si>
-    <t>VN0006</t>
-  </si>
-  <si>
-    <t>VN0007</t>
+    <t>VN0012</t>
   </si>
 </sst>
 </file>
@@ -448,7 +436,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,7 +489,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="2">
-        <v>45594.375</v>
+        <v>45635.375</v>
       </c>
       <c r="D2">
         <v>90</v>
@@ -523,120 +511,16 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45625.375</v>
-      </c>
-      <c r="D3">
-        <v>90</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>1490000</v>
-      </c>
-      <c r="H3">
-        <v>2000000</v>
-      </c>
-      <c r="I3">
-        <v>50000000</v>
-      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2">
-        <v>45626.375</v>
-      </c>
-      <c r="D4">
-        <v>90</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>1490000</v>
-      </c>
-      <c r="H4">
-        <v>2000000</v>
-      </c>
-      <c r="I4">
-        <v>50000000</v>
-      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2">
-        <v>45627.375</v>
-      </c>
-      <c r="D5">
-        <v>90</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>1490000</v>
-      </c>
-      <c r="H5">
-        <v>2000000</v>
-      </c>
-      <c r="I5">
-        <v>50000000</v>
-      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2">
-        <v>45628.375</v>
-      </c>
-      <c r="D6">
-        <v>90</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>1490000</v>
-      </c>
-      <c r="H6">
-        <v>2000000</v>
-      </c>
-      <c r="I6">
-        <v>50000000</v>
-      </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>

</xml_diff>

<commit_message>
add validate + email send booking
</commit_message>
<xml_diff>
--- a/AirlinesReservationSystem/uploads/flight_ticket_class_data.xlsx
+++ b/AirlinesReservationSystem/uploads/flight_ticket_class_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FBT\Kì 8\PRN231\PRN231Fall2024_SE1714_Group5_ARS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341420CC-6F34-46BA-942E-B696453FB151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DA5394-EDFF-4115-B1C0-81C591921CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>FlightNumber</t>
   </si>
@@ -58,7 +58,13 @@
     <t>VN4567</t>
   </si>
   <si>
-    <t>VN0012</t>
+    <t>VN001000</t>
+  </si>
+  <si>
+    <t>VN001001</t>
+  </si>
+  <si>
+    <t>VN001002</t>
   </si>
 </sst>
 </file>
@@ -436,7 +442,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,10 +517,62 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C3" s="2"/>
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45635.458333333336</v>
+      </c>
+      <c r="D3">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>1490000</v>
+      </c>
+      <c r="H3">
+        <v>2000000</v>
+      </c>
+      <c r="I3">
+        <v>50000000</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C4" s="2"/>
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45635.020833333336</v>
+      </c>
+      <c r="D4">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>1490000</v>
+      </c>
+      <c r="H4">
+        <v>2000000</v>
+      </c>
+      <c r="I4">
+        <v>50000000</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>

</xml_diff>

<commit_message>
fix airplane fe + fix passenger fe be
</commit_message>
<xml_diff>
--- a/AirlinesReservationSystem/uploads/flight_ticket_class_data.xlsx
+++ b/AirlinesReservationSystem/uploads/flight_ticket_class_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FBT\Kì 8\PRN231\PRN231Fall2024_SE1714_Group5_ARS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C475780C-AA86-4313-8D0D-BD9523D88FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273A8D44-5364-4360-9196-BFAD674E74A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,16 +49,16 @@
     <t>FirstClassPrice</t>
   </si>
   <si>
-    <t>Tan Son Nhat International Airport</t>
-  </si>
-  <si>
     <t>Noi Bai International Airport</t>
   </si>
   <si>
-    <t>VN4567</t>
-  </si>
-  <si>
-    <t>VN0010098</t>
+    <t>Da Nang International Airport</t>
+  </si>
+  <si>
+    <t>QH3456</t>
+  </si>
+  <si>
+    <t>QH1111</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,31 +483,31 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" s="2">
-        <v>45609.125</v>
+        <v>45602.333333333336</v>
       </c>
       <c r="D2">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
       <c r="G2">
-        <v>1490000</v>
+        <v>1990000</v>
       </c>
       <c r="H2">
-        <v>2000000</v>
+        <v>3400000</v>
       </c>
       <c r="I2">
-        <v>50000000</v>
+        <v>80000000</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix validate excel + add payment success
</commit_message>
<xml_diff>
--- a/AirlinesReservationSystem/uploads/flight_ticket_class_data.xlsx
+++ b/AirlinesReservationSystem/uploads/flight_ticket_class_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FBT\Kì 8\PRN231\PRN231Fall2024_SE1714_Group5_ARS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273A8D44-5364-4360-9196-BFAD674E74A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8076CA6-EA08-4141-BC42-2284D1F9F7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,10 +55,10 @@
     <t>Da Nang International Airport</t>
   </si>
   <si>
-    <t>QH3456</t>
-  </si>
-  <si>
     <t>QH1111</t>
+  </si>
+  <si>
+    <t>QH4444</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,13 +483,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="2">
-        <v>45602.333333333336</v>
+        <v>45602.833333333336</v>
       </c>
       <c r="D2">
         <v>75</v>

</xml_diff>